<commit_message>
Planning update & kappa kart terrain
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enra\Documents\KoolKappaKlan\Concept\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliek\OneDrive\Documenten\TeamSpirit\Concept\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2221,7 +2221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -2491,6 +2491,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2526,6 +2543,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -10600,8 +10634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" topLeftCell="K31" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12279,6 +12313,12 @@
         <v>325</v>
       </c>
       <c r="V43" s="14"/>
+      <c r="W43" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="X43" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="Y43" s="14"/>
       <c r="Z43" s="27"/>
       <c r="AA43" s="16"/>
@@ -12343,6 +12383,12 @@
         <v>327</v>
       </c>
       <c r="V44" s="14"/>
+      <c r="W44" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="X44" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="Y44" s="14"/>
       <c r="Z44" s="27"/>
       <c r="AA44" s="16"/>
@@ -12401,8 +12447,12 @@
       <c r="U45" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="W45" s="8"/>
-      <c r="X45" s="8"/>
+      <c r="W45" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="X45" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="Z45" s="27"/>
       <c r="AA45" s="16"/>
       <c r="AB45" s="16"/>
@@ -12463,6 +12513,9 @@
         <v>343</v>
       </c>
       <c r="V46" s="14"/>
+      <c r="W46" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="Y46" s="14"/>
       <c r="Z46" s="27"/>
       <c r="AA46" s="16"/>
@@ -12518,6 +12571,9 @@
         <v>98</v>
       </c>
       <c r="V47" s="14"/>
+      <c r="W47" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="Y47" s="14"/>
       <c r="Z47" s="27"/>
       <c r="AA47" s="16"/>
@@ -12573,6 +12629,9 @@
         <v>97</v>
       </c>
       <c r="V48" s="14"/>
+      <c r="W48" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="Y48" s="14"/>
       <c r="Z48" s="27"/>
       <c r="AA48" s="16"/>
@@ -12625,6 +12684,9 @@
         <v>96</v>
       </c>
       <c r="V49" s="14"/>
+      <c r="W49" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="Y49" s="14"/>
       <c r="Z49" s="27"/>
       <c r="AA49" s="16"/>
@@ -12677,6 +12739,9 @@
         <v>564</v>
       </c>
       <c r="V50" s="14"/>
+      <c r="W50" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="Y50" s="14"/>
       <c r="Z50" s="27"/>
       <c r="AA50" s="16"/>
@@ -12729,6 +12794,9 @@
         <v>158</v>
       </c>
       <c r="V51" s="14"/>
+      <c r="W51" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="Y51" s="14"/>
       <c r="Z51" s="27"/>
       <c r="AA51" s="16"/>
@@ -13033,9 +13101,6 @@
       <c r="Q57" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="R57" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="S57" s="14"/>
       <c r="T57" s="8" t="s">
         <v>651</v>
@@ -13081,9 +13146,6 @@
       <c r="P58" s="14"/>
       <c r="Q58" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="R58" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="S58" s="14"/>
       <c r="V58" s="14"/>
@@ -13124,9 +13186,6 @@
       <c r="P59" s="14"/>
       <c r="Q59" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="R59" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="S59" s="14"/>
       <c r="V59" s="14"/>
@@ -13330,9 +13389,6 @@
         <v>192</v>
       </c>
       <c r="V64" s="14"/>
-      <c r="W64" s="8" t="s">
-        <v>102</v>
-      </c>
       <c r="Y64" s="14"/>
       <c r="Z64" s="27"/>
       <c r="AA64" s="16"/>
@@ -13389,9 +13445,7 @@
       <c r="U65" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="W65" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="W65" s="8"/>
       <c r="X65" s="8"/>
       <c r="Z65" s="27"/>
       <c r="AA65" s="16"/>
@@ -13447,9 +13501,7 @@
       <c r="U66" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="W66" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="W66" s="8"/>
       <c r="X66" s="8"/>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
@@ -13484,9 +13536,7 @@
       <c r="U67" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="W67" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="W67" s="8"/>
       <c r="X67" s="8"/>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
@@ -13519,9 +13569,7 @@
         <v>290</v>
       </c>
       <c r="U68" s="8"/>
-      <c r="W68" s="8" t="s">
-        <v>104</v>
-      </c>
+      <c r="W68" s="8"/>
       <c r="X68" s="8"/>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
@@ -13552,9 +13600,7 @@
         <v>291</v>
       </c>
       <c r="U69" s="8"/>
-      <c r="W69" s="8" t="s">
-        <v>105</v>
-      </c>
+      <c r="W69" s="8"/>
       <c r="X69" s="8"/>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
@@ -13581,9 +13627,7 @@
         <v>727</v>
       </c>
       <c r="U70" s="8"/>
-      <c r="W70" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="W70" s="8"/>
       <c r="X70" s="8"/>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
@@ -13608,9 +13652,7 @@
         <v>725</v>
       </c>
       <c r="U71" s="8"/>
-      <c r="W71" s="8" t="s">
-        <v>109</v>
-      </c>
+      <c r="W71" s="8"/>
       <c r="X71" s="8"/>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
@@ -13635,9 +13677,7 @@
         <v>723</v>
       </c>
       <c r="U72" s="8"/>
-      <c r="W72" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="W72" s="8"/>
       <c r="X72" s="8"/>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>